<commit_message>
Data from excel file practice
</commit_message>
<xml_diff>
--- a/PlaywrightExcel.xlsx
+++ b/PlaywrightExcel.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -36,52 +31,52 @@
     <t>Vaibhav</t>
   </si>
   <si>
-    <t>Shivam</t>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Sachin</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
   <si>
     <t>Ankul</t>
   </si>
   <si>
+    <t>Civil</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
     <t>Prashant</t>
   </si>
   <si>
+    <t>EC</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
     <t>Ajeet</t>
   </si>
   <si>
+    <t>EE</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
     <t>Divyam</t>
   </si>
   <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t>ME</t>
-  </si>
-  <si>
-    <t>Civil</t>
-  </si>
-  <si>
-    <t>EC</t>
-  </si>
-  <si>
-    <t>EE</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
   </si>
 </sst>
 </file>
@@ -90,11 +85,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -399,18 +394,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.35" customHeight="1"/>
   <cols>
-    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -424,85 +419,88 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E2">
         <v>912367121</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E3">
         <v>7148186412</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
       </c>
       <c r="E4">
         <v>23124121</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E5">
         <v>12312432</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E6">
         <v>254364523</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E7">
         <v>543632523</v>

</xml_diff>